<commit_message>
Interest evaluation for one user is implemented
</commit_message>
<xml_diff>
--- a/Viewer_Describing_Service/src/main/resources/files/Centroids.xlsx
+++ b/Viewer_Describing_Service/src/main/resources/files/Centroids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/polina/IdeaProjects/Advertisement-Selecting/Viewer_Describing_Service/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBE6701F-EDFF-FF43-9D16-9A1E9A61A6CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90EA87E-3430-684C-B2F1-0F508596C117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="2460" windowWidth="26640" windowHeight="14420" xr2:uid="{933D0281-209D-AB40-A821-1C593A2B8E22}"/>
+    <workbookView xWindow="5780" yWindow="8120" windowWidth="22740" windowHeight="8760" xr2:uid="{933D0281-209D-AB40-A821-1C593A2B8E22}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -196,11 +196,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -226,6 +235,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -543,7 +562,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K10" sqref="D2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,35 +606,35 @@
       <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>27.5</v>
+      <c r="B2" s="5">
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="E2" s="5">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
         <v>0</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
-        <v>8.5224999999999995E-2</v>
+      <c r="H2" s="4">
+        <v>0.98462000000000005</v>
       </c>
       <c r="I2" s="5">
-        <v>0.9093</v>
+        <v>1.5375E-2</v>
       </c>
       <c r="J2" s="5">
-        <v>2.1250000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5">
-        <v>7.4999999999999993E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -623,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>56</v>
+        <v>53.75</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>12</v>
@@ -632,24 +651,24 @@
         <v>3.5E-4</v>
       </c>
       <c r="E3" s="8">
-        <v>3.0249999999999999E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="F3" s="8">
-        <v>4.0000000000000002E-4</v>
+        <v>3.5E-4</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
       </c>
       <c r="H3" s="8">
-        <v>0.19259999999999999</v>
+        <v>3.95E-2</v>
       </c>
       <c r="I3" s="8">
-        <v>0.72724999999999995</v>
+        <v>0.92095000000000005</v>
       </c>
       <c r="J3" s="8">
-        <v>4.8899999999999999E-2</v>
-      </c>
-      <c r="K3" s="8">
+        <v>3.32E-2</v>
+      </c>
+      <c r="K3" s="9">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
@@ -658,16 +677,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>40</v>
+        <v>31.536999999999999</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7">
-        <v>0</v>
+      <c r="D4" s="10">
+        <v>6.4814799999999995E-5</v>
       </c>
       <c r="E4" s="8">
-        <v>3.6333300000000002E-3</v>
+        <v>3.2407400000000002E-3</v>
       </c>
       <c r="F4" s="7">
         <v>0</v>
@@ -676,16 +695,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="8">
-        <v>0.19800000000000001</v>
+        <v>7.4907400000000001E-3</v>
       </c>
       <c r="I4" s="8">
-        <v>0.79636700000000005</v>
+        <v>0.984676</v>
       </c>
       <c r="J4" s="8">
-        <v>1.8E-3</v>
+        <v>3.9444399999999996E-3</v>
       </c>
       <c r="K4" s="7">
-        <v>0</v>
+        <v>3.9814800000000002E-4</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -693,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>47</v>
+        <v>43.332999999999998</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
@@ -702,22 +721,22 @@
         <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>5.7000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
       </c>
       <c r="H5" s="8">
-        <v>0.33229999999999998</v>
+        <v>0.98462499999999997</v>
       </c>
       <c r="I5" s="8">
-        <v>0.66080000000000005</v>
+        <v>1.5375E-2</v>
       </c>
       <c r="J5" s="8">
-        <v>6.9999999999999999E-4</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7">
         <v>0</v>
@@ -728,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>33</v>
+        <v>37.5</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>12</v>
@@ -737,33 +756,33 @@
         <v>0</v>
       </c>
       <c r="E6" s="8">
-        <v>2.4199999999999999E-2</v>
+        <v>1.925E-2</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
       </c>
       <c r="H6" s="8">
-        <v>0.51959999999999995</v>
+        <v>0.36925000000000002</v>
       </c>
       <c r="I6" s="8">
-        <v>0.4556</v>
+        <v>0.60975000000000001</v>
       </c>
       <c r="J6" s="8">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="K6" s="7">
-        <v>0</v>
+        <v>1.25E-4</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
-        <v>24</v>
+      <c r="B7" s="11">
+        <v>40</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>11</v>
@@ -772,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="8">
-        <v>5.0666699999999997E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -781,13 +800,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>1E-4</v>
+        <v>0.40949999999999998</v>
       </c>
       <c r="I7" s="8">
-        <v>0.98939999999999995</v>
+        <v>0.58950000000000002</v>
       </c>
       <c r="J7" s="8">
-        <v>5.2666700000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="7">
         <v>0</v>
@@ -798,16 +817,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>36</v>
+        <v>35.125</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7">
         <v>0</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>6.4374999999999996E-3</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -816,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="H8" s="8">
-        <v>0.97699999999999998</v>
+        <v>2.7499999999999998E-3</v>
       </c>
       <c r="I8" s="8">
-        <v>2.3E-2</v>
+        <v>0.98712500000000003</v>
       </c>
       <c r="J8" s="7">
-        <v>0</v>
+        <v>3.375E-3</v>
       </c>
       <c r="K8" s="7">
         <v>0</v>
@@ -833,51 +852,51 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>1.4E-3</v>
+        <v>0.502</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
       </c>
       <c r="H9" s="7">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I9" s="8">
-        <v>0.98329999999999995</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="J9" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K9" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>8</v>
       </c>
       <c r="B10" s="8">
-        <v>36.769199999999998</v>
+        <v>37.444400000000002</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8">
-        <v>2.30769E-4</v>
+        <v>0</v>
       </c>
       <c r="E10" s="8">
-        <v>2.3076899999999998E-3</v>
+        <v>1.5666699999999999E-2</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -885,17 +904,17 @@
       <c r="G10" s="7">
         <v>0</v>
       </c>
-      <c r="H10" s="8">
-        <v>8.46154E-4</v>
+      <c r="H10" s="12">
+        <v>0.62988900000000003</v>
       </c>
       <c r="I10" s="8">
-        <v>0.99350000000000005</v>
+        <v>0.33177800000000002</v>
       </c>
       <c r="J10" s="8">
-        <v>1.2692300000000001E-3</v>
+        <v>2.2222200000000001E-2</v>
       </c>
       <c r="K10" s="8">
-        <v>1.6538499999999999E-3</v>
+        <v>2.22222E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>